<commit_message>
CP03ISSM Cal and Ingest Sheets
Correction made to Cal and Ingest reference designators
Added hydrogen sensors Calibration sheets
Corrected LAT LON format on Cal sheet
</commit_message>
<xml_diff>
--- a/CP03ISSM/Omaha_Cal_Info_CP03ISSM_00002.xlsx
+++ b/CP03ISSM/Omaha_Cal_Info_CP03ISSM_00002.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25823"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="2740" windowWidth="34560" windowHeight="18000" tabRatio="766"/>
+    <workbookView xWindow="300" yWindow="2745" windowWidth="34560" windowHeight="16440" tabRatio="766"/>
   </bookViews>
   <sheets>
     <sheet name="Moorings" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="ACS130_CC_taarray" sheetId="5" r:id="rId5"/>
     <sheet name="ACS130_CC_tcarray" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="686" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="689" uniqueCount="202">
   <si>
     <t>Ref Des</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Calibration Cofficient Value</t>
-  </si>
-  <si>
-    <t>CP03ISSM-SBD11-01-MOPAKO000</t>
   </si>
   <si>
     <t>CP03ISSM-00001-MOPAK</t>
@@ -437,9 +434,6 @@
     <t>CC_eb620</t>
   </si>
   <si>
-    <t>No Calibration Cofficient</t>
-  </si>
-  <si>
     <t>CP03ISSM-SBC11-00-CPMENG000</t>
   </si>
   <si>
@@ -634,16 +628,30 @@
   <si>
     <t>26-1329</t>
   </si>
+  <si>
+    <t>CP03ISSM-SBD11-01-MOPAK0000</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00001-SBD11-02-HYDGN0000</t>
+  </si>
+  <si>
+    <t>CP03ISSM-00001-SBD12-03-HYDGN0000</t>
+  </si>
+  <si>
+    <t>40°21.5667'N</t>
+  </si>
+  <si>
+    <t>70°53.1167'W</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
-    <numFmt numFmtId="165" formatCode="d\-mmm\-yy;@"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -886,7 +894,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="19" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -898,7 +906,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="19" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -914,7 +922,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="4" xfId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,6 +1148,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1468,23 +1481,25 @@
   <dimension ref="A1:AMK2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="1"/>
-    <col min="2" max="2" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.33203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10" style="2" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="3"/>
-    <col min="6" max="6" width="8.83203125" style="2"/>
-    <col min="7" max="10" width="8.83203125" style="1"/>
-    <col min="11" max="11" width="35.5" style="1" customWidth="1"/>
-    <col min="12" max="1025" width="8.83203125" style="1"/>
+    <col min="5" max="5" width="8.85546875" style="3"/>
+    <col min="6" max="6" width="8.85546875" style="2"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" style="1" customWidth="1"/>
+    <col min="9" max="10" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="35.42578125" style="1" customWidth="1"/>
+    <col min="12" max="1025" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="9" customFormat="1" ht="42">
+    <row r="1" spans="1:1025" s="9" customFormat="1" ht="38.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1524,7 +1539,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C2" s="11">
         <v>2</v>
@@ -1536,20 +1551,20 @@
         <v>3.9583333333333331E-2</v>
       </c>
       <c r="F2" s="12"/>
-      <c r="G2" s="10">
-        <v>40.359383333333334</v>
-      </c>
-      <c r="H2" s="10">
-        <v>-70.885300000000001</v>
+      <c r="G2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>201</v>
       </c>
       <c r="I2" s="10">
         <v>97</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="K2" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="L2" s="23"/>
       <c r="M2" s="23"/>
@@ -2579,27 +2594,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMK189"/>
+  <dimension ref="A1:AMK194"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="17.5" style="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5" style="14" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" style="14" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="14" customWidth="1"/>
     <col min="4" max="4" width="19" style="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="46.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="55.6640625" style="14" customWidth="1"/>
-    <col min="8" max="1025" width="8.83203125" style="14"/>
+    <col min="5" max="5" width="39.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="46.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="55.7109375" style="14" customWidth="1"/>
+    <col min="8" max="1025" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1024" s="16" customFormat="1" ht="28">
+    <row r="1" spans="1:1024" s="16" customFormat="1" ht="25.5">
       <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
@@ -3650,21 +3665,21 @@
     </row>
     <row r="3" spans="1:1024">
       <c r="A3" s="14" t="s">
-        <v>16</v>
+        <v>197</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C3" s="14">
         <v>2</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3"/>
       <c r="F3"/>
       <c r="G3" s="19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -4684,38 +4699,41 @@
       <c r="AMI3"/>
       <c r="AMJ3"/>
     </row>
-    <row r="5" spans="1:1024" s="27" customFormat="1">
+    <row r="5" spans="1:1024" s="27" customFormat="1" ht="12.75">
       <c r="A5" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C5" s="27">
         <v>2</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="7" spans="1:1024">
       <c r="A7" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C7" s="14">
         <v>2</v>
       </c>
       <c r="D7" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="28">
         <v>40.359383333333334</v>
       </c>
       <c r="G7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H7"/>
       <c r="I7"/>
@@ -5737,25 +5755,25 @@
     </row>
     <row r="8" spans="1:1024">
       <c r="A8" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C8" s="14">
         <v>2</v>
       </c>
       <c r="D8" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="28">
         <v>-70.885300000000001</v>
       </c>
       <c r="G8" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H8"/>
       <c r="I8"/>
@@ -6777,25 +6795,25 @@
     </row>
     <row r="9" spans="1:1024">
       <c r="A9" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C9" s="14">
         <v>2</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="28">
         <v>1.0668</v>
       </c>
       <c r="G9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H9"/>
       <c r="I9"/>
@@ -7817,25 +7835,25 @@
     </row>
     <row r="10" spans="1:1024">
       <c r="A10" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C10" s="14">
         <v>2</v>
       </c>
       <c r="D10" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="28">
         <v>4.2926000000000002</v>
       </c>
       <c r="G10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H10"/>
       <c r="I10"/>
@@ -8857,25 +8875,25 @@
     </row>
     <row r="11" spans="1:1024">
       <c r="A11" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C11" s="14">
         <v>2</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="28">
         <v>4.2926000000000002</v>
       </c>
       <c r="G11" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H11"/>
       <c r="I11"/>
@@ -9897,25 +9915,25 @@
     </row>
     <row r="12" spans="1:1024">
       <c r="A12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C12" s="14">
         <v>2</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="28">
         <v>4.7497999999999996</v>
       </c>
       <c r="G12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H12"/>
       <c r="I12"/>
@@ -10937,25 +10955,25 @@
     </row>
     <row r="13" spans="1:1024">
       <c r="A13" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C13" s="14">
         <v>2</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F13" s="32">
         <v>1</v>
       </c>
       <c r="G13" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H13"/>
       <c r="I13"/>
@@ -11977,25 +11995,25 @@
     </row>
     <row r="14" spans="1:1024">
       <c r="A14" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C14" s="14">
         <v>2</v>
       </c>
       <c r="D14" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="32">
         <v>1</v>
       </c>
       <c r="G14" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H14"/>
       <c r="I14"/>
@@ -13017,25 +13035,25 @@
     </row>
     <row r="15" spans="1:1024">
       <c r="A15" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C15" s="14">
         <v>2</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F15" s="32">
         <v>600</v>
       </c>
       <c r="G15" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H15"/>
       <c r="I15"/>
@@ -15081,34 +15099,37 @@
       <c r="AMI16"/>
       <c r="AMJ16"/>
     </row>
-    <row r="17" spans="1:1024" s="27" customFormat="1">
+    <row r="17" spans="1:1024" s="27" customFormat="1" ht="12.75">
       <c r="A17" s="25" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>158</v>
       </c>
       <c r="C17" s="27">
         <v>2</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:1024">
       <c r="A19" s="14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" s="14">
         <v>2</v>
       </c>
       <c r="D19" s="28" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E19"/>
       <c r="F19"/>
       <c r="G19" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
@@ -17156,25 +17177,24 @@
     </row>
     <row r="21" spans="1:1024">
       <c r="A21" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C21" s="14">
         <v>2</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F21" s="28">
         <v>40.359383333333334</v>
       </c>
       <c r="G21"/>
-      <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -18194,25 +18214,24 @@
     </row>
     <row r="22" spans="1:1024">
       <c r="A22" s="14" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C22" s="14">
         <v>2</v>
       </c>
       <c r="D22" s="28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F22" s="28">
         <v>-70.885300000000001</v>
       </c>
       <c r="G22"/>
-      <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -19238,7 +19257,6 @@
       <c r="E23"/>
       <c r="F23" s="29"/>
       <c r="G23"/>
-      <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -20258,25 +20276,24 @@
     </row>
     <row r="24" spans="1:1024">
       <c r="A24" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C24" s="14">
         <v>2</v>
       </c>
       <c r="D24" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F24" s="28">
         <v>40.359383333333334</v>
       </c>
       <c r="G24"/>
-      <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -21296,25 +21313,24 @@
     </row>
     <row r="25" spans="1:1024">
       <c r="A25" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C25" s="14">
         <v>2</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F25" s="28">
         <v>-70.885300000000001</v>
       </c>
       <c r="G25"/>
-      <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -22340,7 +22356,6 @@
       <c r="E26"/>
       <c r="F26" s="29"/>
       <c r="G26"/>
-      <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -23360,25 +23375,24 @@
     </row>
     <row r="27" spans="1:1024">
       <c r="A27" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C27" s="14">
         <v>2</v>
       </c>
       <c r="D27" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F27" s="28">
         <v>17533</v>
       </c>
       <c r="G27"/>
-      <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -24398,25 +24412,24 @@
     </row>
     <row r="28" spans="1:1024">
       <c r="A28" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C28" s="14">
         <v>2</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E28" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="28">
         <v>101</v>
       </c>
       <c r="G28"/>
-      <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -25436,25 +25449,24 @@
     </row>
     <row r="29" spans="1:1024">
       <c r="A29" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C29" s="14">
         <v>2</v>
       </c>
       <c r="D29" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E29" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F29" s="28">
         <v>2229</v>
       </c>
       <c r="G29"/>
-      <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -26474,25 +26486,24 @@
     </row>
     <row r="30" spans="1:1024">
       <c r="A30" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C30" s="14">
         <v>2</v>
       </c>
       <c r="D30" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E30" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F30" s="28">
         <v>38502</v>
       </c>
       <c r="G30"/>
-      <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -27512,25 +27523,24 @@
     </row>
     <row r="31" spans="1:1024">
       <c r="A31" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C31" s="14">
         <v>2</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E31" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F31" s="33">
         <v>0</v>
       </c>
       <c r="G31"/>
-      <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -28550,25 +28560,24 @@
     </row>
     <row r="32" spans="1:1024">
       <c r="A32" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C32" s="14">
         <v>2</v>
       </c>
       <c r="D32" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F32" s="33">
         <v>1</v>
       </c>
       <c r="G32"/>
-      <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -29588,27 +29597,26 @@
     </row>
     <row r="33" spans="1:1024">
       <c r="A33" s="14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C33" s="14">
         <v>2</v>
       </c>
       <c r="D33" s="28" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F33" s="32">
         <v>35</v>
       </c>
       <c r="G33" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H33"/>
+        <v>26</v>
+      </c>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -30634,7 +30642,6 @@
       <c r="E34"/>
       <c r="F34"/>
       <c r="G34"/>
-      <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -31654,25 +31661,24 @@
     </row>
     <row r="35" spans="1:1024">
       <c r="A35" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C35" s="14">
         <v>2</v>
       </c>
       <c r="D35" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E35" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F35" s="28">
         <v>17533</v>
       </c>
       <c r="G35"/>
-      <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -32692,25 +32698,24 @@
     </row>
     <row r="36" spans="1:1024">
       <c r="A36" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B36" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C36" s="14">
         <v>2</v>
       </c>
       <c r="D36" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F36" s="28">
         <v>101</v>
       </c>
       <c r="G36"/>
-      <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
@@ -33730,25 +33735,24 @@
     </row>
     <row r="37" spans="1:1024">
       <c r="A37" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B37" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C37" s="14">
         <v>2</v>
       </c>
       <c r="D37" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E37" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F37" s="28">
         <v>2229</v>
       </c>
       <c r="G37"/>
-      <c r="H37"/>
       <c r="I37"/>
       <c r="J37"/>
       <c r="K37"/>
@@ -34768,25 +34772,24 @@
     </row>
     <row r="38" spans="1:1024">
       <c r="A38" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B38" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C38" s="14">
         <v>2</v>
       </c>
       <c r="D38" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F38" s="28">
         <v>38502</v>
       </c>
       <c r="G38"/>
-      <c r="H38"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38"/>
@@ -35806,25 +35809,24 @@
     </row>
     <row r="39" spans="1:1024">
       <c r="A39" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C39" s="14">
         <v>2</v>
       </c>
       <c r="D39" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F39" s="33">
         <v>0</v>
       </c>
       <c r="G39"/>
-      <c r="H39"/>
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39"/>
@@ -36844,25 +36846,24 @@
     </row>
     <row r="40" spans="1:1024">
       <c r="A40" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B40" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" s="14">
         <v>2</v>
       </c>
       <c r="D40" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F40" s="33">
         <v>1</v>
       </c>
       <c r="G40"/>
-      <c r="H40"/>
       <c r="I40"/>
       <c r="J40"/>
       <c r="K40"/>
@@ -37882,27 +37883,26 @@
     </row>
     <row r="41" spans="1:1024">
       <c r="A41" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C41" s="14">
         <v>2</v>
       </c>
       <c r="D41" s="28" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E41" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F41" s="32">
         <v>35</v>
       </c>
       <c r="G41" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="H41"/>
+        <v>26</v>
+      </c>
       <c r="I41"/>
       <c r="J41"/>
       <c r="K41"/>
@@ -38928,7 +38928,6 @@
       <c r="E42"/>
       <c r="F42"/>
       <c r="G42"/>
-      <c r="H42"/>
       <c r="I42"/>
       <c r="J42"/>
       <c r="K42"/>
@@ -39948,25 +39947,24 @@
     </row>
     <row r="43" spans="1:1024">
       <c r="A43" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B43" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C43" s="14">
         <v>2</v>
       </c>
       <c r="D43" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E43" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F43" s="28" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G43"/>
-      <c r="H43"/>
       <c r="I43"/>
       <c r="J43"/>
       <c r="K43"/>
@@ -40986,25 +40984,24 @@
     </row>
     <row r="44" spans="1:1024">
       <c r="A44" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C44" s="14">
         <v>2</v>
       </c>
       <c r="D44" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F44" s="28" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G44"/>
-      <c r="H44"/>
       <c r="I44"/>
       <c r="J44"/>
       <c r="K44"/>
@@ -42024,19 +42021,19 @@
     </row>
     <row r="45" spans="1:1024">
       <c r="A45" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C45" s="14">
         <v>2</v>
       </c>
       <c r="D45" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F45" s="28">
         <v>19.5</v>
@@ -43062,22 +43059,22 @@
     </row>
     <row r="46" spans="1:1024">
       <c r="A46" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B46" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C46" s="14">
         <v>2</v>
       </c>
       <c r="D46" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F46" s="28" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="G46"/>
       <c r="H46"/>
@@ -44100,22 +44097,22 @@
     </row>
     <row r="47" spans="1:1024">
       <c r="A47" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B47" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" s="14">
         <v>2</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F47" s="28" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G47"/>
       <c r="H47"/>
@@ -45138,22 +45135,22 @@
     </row>
     <row r="48" spans="1:1024">
       <c r="A48" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B48" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C48" s="14">
         <v>2</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E48" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F48" s="28" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="G48"/>
       <c r="H48"/>
@@ -46176,22 +46173,22 @@
     </row>
     <row r="49" spans="1:1024">
       <c r="A49" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B49" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C49" s="14">
         <v>2</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E49" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F49" s="28" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G49"/>
       <c r="H49"/>
@@ -47212,24 +47209,24 @@
       <c r="AMI49"/>
       <c r="AMJ49"/>
     </row>
-    <row r="50" spans="1:1024" s="20" customFormat="1">
+    <row r="50" spans="1:1024" s="20" customFormat="1" ht="12.75">
       <c r="A50" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B50" s="20" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C50" s="20">
         <v>2</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F50" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="51" spans="1:1024">
@@ -47243,61 +47240,61 @@
     </row>
     <row r="52" spans="1:1024">
       <c r="A52" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B52" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" s="14">
         <v>2</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="G52"/>
     </row>
     <row r="53" spans="1:1024">
       <c r="A53" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="14">
         <v>2</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G53"/>
     </row>
     <row r="54" spans="1:1024">
       <c r="A54" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" s="14">
         <v>2</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F54" s="28">
         <v>17.7</v>
@@ -47306,106 +47303,106 @@
     </row>
     <row r="55" spans="1:1024">
       <c r="A55" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B55" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C55" s="14">
         <v>2</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E55" s="14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G55"/>
     </row>
     <row r="56" spans="1:1024">
       <c r="A56" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B56" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C56" s="14">
         <v>2</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E56" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="G56"/>
     </row>
     <row r="57" spans="1:1024">
       <c r="A57" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B57" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="14">
         <v>2</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E57" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="G57"/>
     </row>
     <row r="58" spans="1:1024">
       <c r="A58" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B58" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C58" s="14">
         <v>2</v>
       </c>
       <c r="D58" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E58" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="G58"/>
     </row>
     <row r="59" spans="1:1024">
       <c r="A59" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B59" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C59" s="14">
         <v>2</v>
       </c>
       <c r="D59" s="28" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E59" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="G59"/>
     </row>
@@ -47420,10 +47417,10 @@
     </row>
     <row r="61" spans="1:1024">
       <c r="A61" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B61" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61" s="14">
         <v>2</v>
@@ -47432,7 +47429,7 @@
         <v>1222</v>
       </c>
       <c r="E61" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F61" s="28">
         <v>64</v>
@@ -47441,10 +47438,10 @@
     </row>
     <row r="62" spans="1:1024">
       <c r="A62" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B62" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C62" s="14">
         <v>2</v>
@@ -47453,7 +47450,7 @@
         <v>1222</v>
       </c>
       <c r="E62" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F62" s="37">
         <v>1.9530000000000002E-6</v>
@@ -47462,10 +47459,10 @@
     </row>
     <row r="63" spans="1:1024">
       <c r="A63" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" s="14">
         <v>2</v>
@@ -47474,7 +47471,7 @@
         <v>1222</v>
       </c>
       <c r="E63" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F63" s="28">
         <v>47</v>
@@ -47483,10 +47480,10 @@
     </row>
     <row r="64" spans="1:1024">
       <c r="A64" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B64" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C64" s="14">
         <v>2</v>
@@ -47495,7 +47492,7 @@
         <v>1222</v>
       </c>
       <c r="E64" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F64" s="28">
         <v>1.21E-2</v>
@@ -47504,10 +47501,10 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B65" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C65" s="14">
         <v>2</v>
@@ -47516,7 +47513,7 @@
         <v>1222</v>
       </c>
       <c r="E65" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F65" s="28">
         <v>44</v>
@@ -47525,10 +47522,10 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B66" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C66" s="14">
         <v>2</v>
@@ -47537,7 +47534,7 @@
         <v>1222</v>
       </c>
       <c r="E66" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F66" s="28">
         <v>9.0399999999999994E-2</v>
@@ -47546,10 +47543,10 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B67" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C67" s="14">
         <v>2</v>
@@ -47558,21 +47555,21 @@
         <v>1222</v>
       </c>
       <c r="E67" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F67" s="34">
         <v>124</v>
       </c>
       <c r="G67" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="A68" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B68" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C68" s="14">
         <v>2</v>
@@ -47581,21 +47578,21 @@
         <v>1222</v>
       </c>
       <c r="E68" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F68" s="34">
         <v>700</v>
       </c>
       <c r="G68" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="A69" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B69" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="14">
         <v>2</v>
@@ -47604,21 +47601,21 @@
         <v>1222</v>
       </c>
       <c r="E69" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F69" s="34">
         <v>1.0760000000000001</v>
       </c>
       <c r="G69" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="A70" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B70" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C70" s="14">
         <v>2</v>
@@ -47627,13 +47624,13 @@
         <v>1222</v>
       </c>
       <c r="E70" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F70" s="34">
         <v>3.9E-2</v>
       </c>
       <c r="G70" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -47647,19 +47644,19 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B72" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C72" s="14">
         <v>2</v>
       </c>
       <c r="D72" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E72" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F72" s="28">
         <v>40.359383333333334</v>
@@ -47668,19 +47665,19 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B73" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C73" s="14">
         <v>2</v>
       </c>
       <c r="D73" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E73" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F73" s="28">
         <v>-70.885300000000001</v>
@@ -47689,19 +47686,19 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B74" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C74" s="14">
         <v>2</v>
       </c>
       <c r="D74" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E74" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F74" s="28">
         <v>1.256273E-3</v>
@@ -47710,19 +47707,19 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B75" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C75" s="14">
         <v>2</v>
       </c>
       <c r="D75" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E75" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F75" s="28">
         <v>2.7381850000000001E-4</v>
@@ -47731,19 +47728,19 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B76" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C76" s="14">
         <v>2</v>
       </c>
       <c r="D76" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E76" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F76" s="28">
         <v>-1.1250199999999999E-6</v>
@@ -47752,19 +47749,19 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C77" s="14">
         <v>2</v>
       </c>
       <c r="D77" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E77" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F77" s="28">
         <v>1.8397970000000001E-7</v>
@@ -47773,19 +47770,19 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C78" s="14">
         <v>2</v>
       </c>
       <c r="D78" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E78" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F78" s="28">
         <v>-65.473010000000002</v>
@@ -47794,19 +47791,19 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B79" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C79" s="14">
         <v>2</v>
       </c>
       <c r="D79" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E79" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F79" s="28">
         <v>52.401969999999999</v>
@@ -47815,341 +47812,344 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B80" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" s="14">
         <v>2</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E80" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F80" s="28">
         <v>-0.52704479999999998</v>
       </c>
       <c r="G80"/>
     </row>
-    <row r="81" spans="1:7">
+    <row r="81" spans="1:8">
       <c r="A81" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B81" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C81" s="14">
         <v>2</v>
       </c>
       <c r="D81" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E81" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F81" s="28">
         <v>509054.5</v>
       </c>
       <c r="G81"/>
     </row>
-    <row r="82" spans="1:7">
+    <row r="82" spans="1:8">
       <c r="A82" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B82" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C82" s="14">
         <v>2</v>
       </c>
       <c r="D82" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E82" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F82" s="28">
         <v>-39.351739999999999</v>
       </c>
       <c r="G82"/>
     </row>
-    <row r="83" spans="1:7">
+    <row r="83" spans="1:8">
       <c r="A83" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B83" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C83" s="14">
         <v>2</v>
       </c>
       <c r="D83" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E83" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F83" s="28">
         <v>0.58878529999999996</v>
       </c>
       <c r="G83"/>
+      <c r="H83"/>
     </row>
-    <row r="84" spans="1:7">
+    <row r="84" spans="1:8">
       <c r="A84" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B84" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C84" s="14">
         <v>2</v>
       </c>
       <c r="D84" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E84" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F84" s="28">
         <v>24.950130000000001</v>
       </c>
       <c r="G84"/>
+      <c r="H84"/>
     </row>
-    <row r="85" spans="1:7">
+    <row r="85" spans="1:8">
       <c r="A85" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B85" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C85" s="14">
         <v>2</v>
       </c>
       <c r="D85" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E85" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F85" s="28">
         <v>-9.7499999999999996E-4</v>
       </c>
       <c r="G85"/>
+      <c r="H85"/>
     </row>
-    <row r="86" spans="1:7">
+    <row r="86" spans="1:8">
       <c r="A86" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B86" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C86" s="14">
         <v>2</v>
       </c>
       <c r="D86" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E86" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F86" s="28">
         <v>0</v>
       </c>
       <c r="G86"/>
     </row>
-    <row r="87" spans="1:7">
+    <row r="87" spans="1:8">
       <c r="A87" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B87" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C87" s="14">
         <v>2</v>
       </c>
       <c r="D87" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E87" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F87" s="28">
         <v>-0.27649109999999999</v>
       </c>
       <c r="G87"/>
     </row>
-    <row r="88" spans="1:7">
+    <row r="88" spans="1:8">
       <c r="A88" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B88" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C88" s="14">
         <v>2</v>
       </c>
       <c r="D88" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E88" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F88" s="28">
         <v>4.674716E-4</v>
       </c>
       <c r="G88"/>
     </row>
-    <row r="89" spans="1:7">
+    <row r="89" spans="1:8">
       <c r="A89" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B89" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C89" s="14">
         <v>2</v>
       </c>
       <c r="D89" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E89" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F89" s="28">
         <v>-4.0824430000000002E-12</v>
       </c>
       <c r="G89"/>
     </row>
-    <row r="90" spans="1:7">
+    <row r="90" spans="1:8">
       <c r="A90" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B90" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C90" s="14">
         <v>2</v>
       </c>
       <c r="D90" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E90" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F90" s="28">
         <v>-0.97573339999999997</v>
       </c>
       <c r="G90"/>
     </row>
-    <row r="91" spans="1:7">
+    <row r="91" spans="1:8">
       <c r="A91" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B91" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C91" s="14">
         <v>2</v>
       </c>
       <c r="D91" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E91" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F91" s="28">
         <v>0.14553940000000001</v>
       </c>
       <c r="G91"/>
     </row>
-    <row r="92" spans="1:7">
+    <row r="92" spans="1:8">
       <c r="A92" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B92" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C92" s="14">
         <v>2</v>
       </c>
       <c r="D92" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E92" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F92" s="28">
         <v>-1.5039409999999999E-4</v>
       </c>
       <c r="G92"/>
     </row>
-    <row r="93" spans="1:7">
+    <row r="93" spans="1:8">
       <c r="A93" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B93" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C93" s="14">
         <v>2</v>
       </c>
       <c r="D93" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E93" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F93" s="28">
         <v>3.1549679999999999E-5</v>
       </c>
       <c r="G93"/>
     </row>
-    <row r="94" spans="1:7">
+    <row r="94" spans="1:8">
       <c r="A94" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B94" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C94" s="14">
         <v>2</v>
       </c>
       <c r="D94" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E94" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F94" s="28">
         <v>-9.5700000000000003E-8</v>
       </c>
       <c r="G94"/>
     </row>
-    <row r="95" spans="1:7">
+    <row r="95" spans="1:8">
       <c r="A95" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B95" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C95" s="14">
         <v>2</v>
       </c>
       <c r="D95" s="28" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E95" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F95" s="28">
         <v>3.2499999999999998E-6</v>
       </c>
       <c r="G95"/>
     </row>
-    <row r="96" spans="1:7">
+    <row r="96" spans="1:8">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -48160,19 +48160,19 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B97" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C97" s="14">
         <v>2</v>
       </c>
       <c r="D97" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E97" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F97" s="28">
         <v>40.359383333333334</v>
@@ -48181,19 +48181,19 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B98" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C98" s="14">
         <v>2</v>
       </c>
       <c r="D98" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E98" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F98" s="28">
         <v>-70.885300000000001</v>
@@ -48202,19 +48202,19 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B99" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C99" s="14">
         <v>2</v>
       </c>
       <c r="D99" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E99" s="14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F99" s="28">
         <v>1.260873E-3</v>
@@ -48223,19 +48223,19 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B100" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C100" s="14">
         <v>2</v>
       </c>
       <c r="D100" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F100" s="28">
         <v>2.7196540000000002E-4</v>
@@ -48244,19 +48244,19 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B101" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C101" s="14">
         <v>2</v>
       </c>
       <c r="D101" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E101" s="14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F101" s="28">
         <v>-9.804536E-7</v>
@@ -48265,19 +48265,19 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B102" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C102" s="14">
         <v>2</v>
       </c>
       <c r="D102" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E102" s="14" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F102" s="28">
         <v>1.780167E-7</v>
@@ -48286,19 +48286,19 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B103" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C103" s="14">
         <v>2</v>
       </c>
       <c r="D103" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E103" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F103" s="28">
         <v>-67.553910000000002</v>
@@ -48307,19 +48307,19 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B104" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C104" s="14">
         <v>2</v>
       </c>
       <c r="D104" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E104" s="14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F104" s="28">
         <v>51.100990000000003</v>
@@ -48328,19 +48328,19 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B105" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C105" s="14">
         <v>2</v>
       </c>
       <c r="D105" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E105" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F105" s="28">
         <v>-0.33188099999999998</v>
@@ -48349,19 +48349,19 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B106" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C106" s="14">
         <v>2</v>
       </c>
       <c r="D106" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E106" s="14" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F106" s="28">
         <v>525416.80000000005</v>
@@ -48370,19 +48370,19 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B107" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C107" s="14">
         <v>2</v>
       </c>
       <c r="D107" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E107" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F107" s="28">
         <v>2.8752270000000002</v>
@@ -48391,19 +48391,19 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B108" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C108" s="14">
         <v>2</v>
       </c>
       <c r="D108" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E108" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F108" s="28">
         <v>-9.0869469999999994E-2</v>
@@ -48412,19 +48412,19 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B109" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C109" s="14">
         <v>2</v>
       </c>
       <c r="D109" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E109" s="14" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F109" s="28">
         <v>25.109629999999999</v>
@@ -48433,19 +48433,19 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B110" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C110" s="14">
         <v>2</v>
       </c>
       <c r="D110" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E110" s="14" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F110" s="28">
         <v>-6.7500000000000004E-4</v>
@@ -48454,19 +48454,19 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B111" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C111" s="14">
         <v>2</v>
       </c>
       <c r="D111" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E111" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F111" s="28">
         <v>0</v>
@@ -48475,19 +48475,19 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B112" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C112" s="14">
         <v>2</v>
       </c>
       <c r="D112" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E112" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F112" s="28">
         <v>3.1207929999999998E-2</v>
@@ -48496,19 +48496,19 @@
     </row>
     <row r="113" spans="1:7">
       <c r="A113" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B113" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C113" s="14">
         <v>2</v>
       </c>
       <c r="D113" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E113" s="14" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F113" s="28">
         <v>1.5466919999999999E-3</v>
@@ -48517,19 +48517,19 @@
     </row>
     <row r="114" spans="1:7">
       <c r="A114" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C114" s="14">
         <v>2</v>
       </c>
       <c r="D114" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E114" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F114" s="28">
         <v>5.5330189999999996E-12</v>
@@ -48538,19 +48538,19 @@
     </row>
     <row r="115" spans="1:7">
       <c r="A115" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B115" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C115" s="14">
         <v>2</v>
       </c>
       <c r="D115" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E115" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F115" s="28">
         <v>-0.97371370000000002</v>
@@ -48559,19 +48559,19 @@
     </row>
     <row r="116" spans="1:7">
       <c r="A116" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B116" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C116" s="14">
         <v>2</v>
       </c>
       <c r="D116" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E116" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F116" s="28">
         <v>0.15092559999999999</v>
@@ -48580,19 +48580,19 @@
     </row>
     <row r="117" spans="1:7">
       <c r="A117" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B117" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C117" s="14">
         <v>2</v>
       </c>
       <c r="D117" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E117" s="14" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F117" s="28">
         <v>-1.5058270000000001E-4</v>
@@ -48601,19 +48601,19 @@
     </row>
     <row r="118" spans="1:7">
       <c r="A118" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B118" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C118" s="14">
         <v>2</v>
       </c>
       <c r="D118" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E118" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F118" s="28">
         <v>3.3778990000000002E-5</v>
@@ -48622,19 +48622,19 @@
     </row>
     <row r="119" spans="1:7">
       <c r="A119" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B119" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C119" s="14">
         <v>2</v>
       </c>
       <c r="D119" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E119" s="14" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F119" s="28">
         <v>-9.5700000000000003E-8</v>
@@ -48643,19 +48643,19 @@
     </row>
     <row r="120" spans="1:7">
       <c r="A120" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B120" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C120" s="14">
         <v>2</v>
       </c>
       <c r="D120" s="28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E120" s="14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F120" s="28">
         <v>3.2499999999999998E-6</v>
@@ -48673,10 +48673,10 @@
     </row>
     <row r="122" spans="1:7">
       <c r="A122" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B122" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C122" s="14">
         <v>2</v>
@@ -48685,7 +48685,7 @@
         <v>130</v>
       </c>
       <c r="E122" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F122" s="28">
         <v>40.359383333333334</v>
@@ -48694,10 +48694,10 @@
     </row>
     <row r="123" spans="1:7">
       <c r="A123" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B123" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C123" s="14">
         <v>2</v>
@@ -48706,7 +48706,7 @@
         <v>130</v>
       </c>
       <c r="E123" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F123" s="28">
         <v>-70.885300000000001</v>
@@ -48715,10 +48715,10 @@
     </row>
     <row r="124" spans="1:7">
       <c r="A124" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B124" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C124" s="14">
         <v>2</v>
@@ -48727,10 +48727,10 @@
         <v>130</v>
       </c>
       <c r="E124" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F124" s="28" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G124"/>
     </row>
@@ -48745,10 +48745,10 @@
     </row>
     <row r="126" spans="1:7">
       <c r="A126" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B126" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C126" s="14">
         <v>2</v>
@@ -48757,7 +48757,7 @@
         <v>225</v>
       </c>
       <c r="E126" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F126" s="28">
         <v>40.359383333333334</v>
@@ -48766,10 +48766,10 @@
     </row>
     <row r="127" spans="1:7">
       <c r="A127" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B127" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C127" s="14">
         <v>2</v>
@@ -48778,7 +48778,7 @@
         <v>225</v>
       </c>
       <c r="E127" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F127" s="28">
         <v>-70.885300000000001</v>
@@ -48787,10 +48787,10 @@
     </row>
     <row r="128" spans="1:7">
       <c r="A128" s="14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B128" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C128" s="14">
         <v>2</v>
@@ -48799,10 +48799,10 @@
         <v>225</v>
       </c>
       <c r="E128" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F128" s="28" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G128"/>
     </row>
@@ -48817,10 +48817,10 @@
     </row>
     <row r="130" spans="1:7">
       <c r="A130" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B130" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C130" s="14">
         <v>2</v>
@@ -48829,21 +48829,21 @@
         <v>270</v>
       </c>
       <c r="E130" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F130" s="32">
         <v>217</v>
       </c>
       <c r="G130" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="131" spans="1:7">
       <c r="A131" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B131" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C131" s="14">
         <v>2</v>
@@ -48852,21 +48852,21 @@
         <v>270</v>
       </c>
       <c r="E131" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F131" s="32">
         <v>240</v>
       </c>
       <c r="G131" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:7">
       <c r="A132" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B132" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C132" s="14">
         <v>2</v>
@@ -48875,7 +48875,7 @@
         <v>270</v>
       </c>
       <c r="E132" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F132" s="28">
         <v>20.059999999999999</v>
@@ -48884,10 +48884,10 @@
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B133" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C133" s="14">
         <v>2</v>
@@ -48896,19 +48896,19 @@
         <v>270</v>
       </c>
       <c r="E133" s="14" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F133" s="36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G133"/>
     </row>
     <row r="134" spans="1:7">
       <c r="A134" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B134" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C134" s="14">
         <v>2</v>
@@ -48917,19 +48917,19 @@
         <v>270</v>
       </c>
       <c r="E134" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F134" s="28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="G134"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B135" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C135" s="14">
         <v>2</v>
@@ -48938,19 +48938,19 @@
         <v>270</v>
       </c>
       <c r="E135" s="14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F135" s="28" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G135"/>
     </row>
     <row r="136" spans="1:7">
       <c r="A136" s="30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B136" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C136" s="14">
         <v>2</v>
@@ -48959,10 +48959,10 @@
         <v>270</v>
       </c>
       <c r="E136" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F136" s="36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="G136"/>
     </row>
@@ -48977,10 +48977,10 @@
     </row>
     <row r="138" spans="1:7">
       <c r="A138" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B138" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C138" s="14">
         <v>2</v>
@@ -48989,19 +48989,19 @@
         <v>273</v>
       </c>
       <c r="E138" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F138" s="28" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G138"/>
     </row>
     <row r="139" spans="1:7">
       <c r="A139" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B139" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C139" s="14">
         <v>2</v>
@@ -49010,19 +49010,19 @@
         <v>273</v>
       </c>
       <c r="E139" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F139" s="28" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G139"/>
     </row>
     <row r="140" spans="1:7">
       <c r="A140" s="30" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="B140" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C140" s="14">
         <v>2</v>
@@ -49031,10 +49031,10 @@
         <v>273</v>
       </c>
       <c r="E140" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F140" s="28" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G140"/>
     </row>
@@ -49049,10 +49049,10 @@
     </row>
     <row r="142" spans="1:7">
       <c r="A142" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B142" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C142" s="14">
         <v>2</v>
@@ -49061,7 +49061,7 @@
         <v>18594</v>
       </c>
       <c r="E142" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F142" s="28">
         <v>97000</v>
@@ -49070,10 +49070,10 @@
     </row>
     <row r="143" spans="1:7">
       <c r="A143" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B143" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C143" s="14">
         <v>2</v>
@@ -49082,7 +49082,7 @@
         <v>18594</v>
       </c>
       <c r="E143" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F143" s="28">
         <v>40.359383333333334</v>
@@ -49091,10 +49091,10 @@
     </row>
     <row r="144" spans="1:7">
       <c r="A144" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B144" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C144" s="14">
         <v>2</v>
@@ -49103,7 +49103,7 @@
         <v>18594</v>
       </c>
       <c r="E144" s="14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F144" s="28">
         <v>-70.885300000000001</v>
@@ -49112,10 +49112,10 @@
     </row>
     <row r="145" spans="1:7">
       <c r="A145" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B145" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C145" s="14">
         <v>2</v>
@@ -49124,7 +49124,7 @@
         <v>18594</v>
       </c>
       <c r="E145" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F145" s="32">
         <v>0.45</v>
@@ -49133,10 +49133,10 @@
     </row>
     <row r="146" spans="1:7">
       <c r="A146" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B146" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C146" s="14">
         <v>2</v>
@@ -49145,7 +49145,7 @@
         <v>18594</v>
       </c>
       <c r="E146" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F146" s="32">
         <v>0.45</v>
@@ -49154,10 +49154,10 @@
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B147" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C147" s="14">
         <v>2</v>
@@ -49166,7 +49166,7 @@
         <v>18594</v>
       </c>
       <c r="E147" s="14" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F147" s="32">
         <v>0.45</v>
@@ -49175,10 +49175,10 @@
     </row>
     <row r="148" spans="1:7">
       <c r="A148" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C148" s="14">
         <v>2</v>
@@ -49187,7 +49187,7 @@
         <v>18594</v>
       </c>
       <c r="E148" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F148" s="32">
         <v>0.45</v>
@@ -49205,19 +49205,19 @@
     </row>
     <row r="150" spans="1:7">
       <c r="A150" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B150" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C150" s="14">
         <v>2</v>
       </c>
       <c r="D150" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E150" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F150" s="28">
         <v>2064.6590000000001</v>
@@ -49226,19 +49226,19 @@
     </row>
     <row r="151" spans="1:7">
       <c r="A151" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B151" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C151" s="14">
         <v>2</v>
       </c>
       <c r="D151" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E151" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F151" s="28">
         <v>14.16356</v>
@@ -49247,19 +49247,19 @@
     </row>
     <row r="152" spans="1:7">
       <c r="A152" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B152" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C152" s="14">
         <v>2</v>
       </c>
       <c r="D152" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E152" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F152" s="28">
         <v>-3193.857</v>
@@ -49268,19 +49268,19 @@
     </row>
     <row r="153" spans="1:7">
       <c r="A153" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B153" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C153" s="14">
         <v>2</v>
       </c>
       <c r="D153" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E153" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F153" s="28">
         <v>1.1655E-2</v>
@@ -49289,19 +49289,19 @@
     </row>
     <row r="154" spans="1:7">
       <c r="A154" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B154" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C154" s="14">
         <v>2</v>
       </c>
       <c r="D154" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E154" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F154" s="28">
         <v>0</v>
@@ -49310,42 +49310,42 @@
     </row>
     <row r="155" spans="1:7">
       <c r="A155" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B155" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C155" s="14">
         <v>2</v>
       </c>
       <c r="D155" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E155" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F155" s="32">
         <v>0</v>
       </c>
       <c r="G155" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="156" spans="1:7">
       <c r="A156" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B156" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C156" s="14">
         <v>2</v>
       </c>
       <c r="D156" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E156" s="14" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F156" s="28">
         <v>-0.2472</v>
@@ -49354,42 +49354,42 @@
     </row>
     <row r="157" spans="1:7">
       <c r="A157" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B157" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C157" s="14">
         <v>2</v>
       </c>
       <c r="D157" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E157" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F157" s="32">
         <v>1</v>
       </c>
       <c r="G157" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="158" spans="1:7">
       <c r="A158" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B158" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C158" s="14">
         <v>2</v>
       </c>
       <c r="D158" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E158" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F158" s="28">
         <v>27.61045</v>
@@ -49398,19 +49398,19 @@
     </row>
     <row r="159" spans="1:7">
       <c r="A159" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B159" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C159" s="14">
         <v>2</v>
       </c>
       <c r="D159" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E159" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F159" s="28">
         <v>0.23627100000000001</v>
@@ -49419,103 +49419,103 @@
     </row>
     <row r="160" spans="1:7">
       <c r="A160" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B160" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C160" s="14">
         <v>2</v>
       </c>
       <c r="D160" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E160" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F160" s="28">
         <v>16.693860000000001</v>
       </c>
       <c r="G160"/>
     </row>
-    <row r="161" spans="1:7">
+    <row r="161" spans="1:8">
       <c r="A161" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B161" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C161" s="14">
         <v>2</v>
       </c>
       <c r="D161" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E161" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F161" s="28">
         <v>32.303669999999997</v>
       </c>
       <c r="G161"/>
     </row>
-    <row r="162" spans="1:7">
+    <row r="162" spans="1:8">
       <c r="A162" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B162" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C162" s="14">
         <v>2</v>
       </c>
       <c r="D162" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E162" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F162" s="28">
         <v>5.8436409999999999</v>
       </c>
       <c r="G162"/>
     </row>
-    <row r="163" spans="1:7">
+    <row r="163" spans="1:8">
       <c r="A163" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B163" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C163" s="14">
         <v>2</v>
       </c>
       <c r="D163" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E163" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F163" s="28">
         <v>-3952.915</v>
       </c>
       <c r="G163"/>
     </row>
-    <row r="164" spans="1:7">
+    <row r="164" spans="1:8">
       <c r="A164" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B164" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C164" s="14">
         <v>2</v>
       </c>
       <c r="D164" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E164" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F164" s="28">
         <f>10377.22</f>
@@ -49523,70 +49523,70 @@
       </c>
       <c r="G164"/>
     </row>
-    <row r="165" spans="1:7">
+    <row r="165" spans="1:8">
       <c r="A165" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C165" s="14">
         <v>2</v>
       </c>
       <c r="D165" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E165" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F165" s="28">
         <v>0</v>
       </c>
       <c r="G165"/>
     </row>
-    <row r="166" spans="1:7">
+    <row r="166" spans="1:8">
       <c r="A166" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B166" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C166" s="14">
         <v>2</v>
       </c>
       <c r="D166" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E166" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F166" s="32">
         <v>2796.2</v>
       </c>
       <c r="G166"/>
     </row>
-    <row r="167" spans="1:7">
+    <row r="167" spans="1:8">
       <c r="A167" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B167" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C167" s="14">
         <v>2</v>
       </c>
       <c r="D167" s="28" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E167" s="14" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F167" s="32">
         <v>41943</v>
       </c>
       <c r="G167"/>
     </row>
-    <row r="168" spans="1:7">
+    <row r="168" spans="1:8">
       <c r="A168"/>
       <c r="B168"/>
       <c r="C168"/>
@@ -49595,181 +49595,184 @@
       <c r="F168"/>
       <c r="G168"/>
     </row>
-    <row r="169" spans="1:7">
+    <row r="169" spans="1:8">
       <c r="A169" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B169" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C169" s="14">
         <v>2</v>
       </c>
       <c r="D169" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E169" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F169" s="28">
         <v>-8.3999999999999995E-3</v>
       </c>
       <c r="G169"/>
     </row>
-    <row r="170" spans="1:7">
+    <row r="170" spans="1:8">
       <c r="A170" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B170" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C170" s="14">
         <v>2</v>
       </c>
       <c r="D170" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E170" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F170" s="28">
         <v>0.91239999999999999</v>
       </c>
       <c r="G170"/>
     </row>
-    <row r="171" spans="1:7">
+    <row r="171" spans="1:8">
       <c r="A171" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B171" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C171" s="14">
         <v>2</v>
       </c>
       <c r="D171" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E171" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F171" s="28">
         <v>-1.958</v>
       </c>
       <c r="G171"/>
     </row>
-    <row r="172" spans="1:7">
+    <row r="172" spans="1:8">
       <c r="A172" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C172" s="14">
         <v>2</v>
       </c>
       <c r="D172" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E172" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F172" s="28">
         <v>14.77</v>
       </c>
       <c r="G172"/>
     </row>
-    <row r="173" spans="1:7">
+    <row r="173" spans="1:8">
       <c r="A173" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B173" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C173" s="14">
         <v>2</v>
       </c>
       <c r="D173" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E173" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F173" s="32">
         <v>19706</v>
       </c>
       <c r="G173" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
-    <row r="174" spans="1:7">
+    <row r="174" spans="1:8">
       <c r="A174" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B174" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C174" s="14">
         <v>2</v>
       </c>
       <c r="D174" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E174" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F174" s="32">
         <v>34</v>
       </c>
       <c r="G174" t="s">
-        <v>174</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H174"/>
     </row>
-    <row r="175" spans="1:7">
+    <row r="175" spans="1:8">
       <c r="A175" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B175" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C175" s="14">
         <v>2</v>
       </c>
       <c r="D175" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E175" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F175" s="32">
         <v>3073</v>
       </c>
       <c r="G175" t="s">
-        <v>174</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H175"/>
     </row>
-    <row r="176" spans="1:7">
+    <row r="176" spans="1:8">
       <c r="A176" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B176" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C176" s="14">
         <v>2</v>
       </c>
       <c r="D176" s="28" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E176" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F176" s="32">
         <v>44327</v>
       </c>
       <c r="G176" t="s">
-        <v>174</v>
-      </c>
+        <v>172</v>
+      </c>
+      <c r="H176"/>
     </row>
     <row r="177" spans="1:1025">
       <c r="A177"/>
@@ -49777,28 +49780,23 @@
       <c r="C177"/>
       <c r="D177" s="29"/>
       <c r="G177"/>
+      <c r="H177"/>
     </row>
     <row r="178" spans="1:1025" s="24" customFormat="1">
-      <c r="A178" s="30" t="s">
-        <v>157</v>
-      </c>
-      <c r="B178" s="17" t="s">
-        <v>158</v>
-      </c>
-      <c r="C178" s="17">
-        <v>2</v>
-      </c>
-      <c r="D178" s="30">
-        <v>55080</v>
-      </c>
       <c r="E178" s="17"/>
       <c r="F178" s="17"/>
-      <c r="G178" s="17" t="s">
-        <v>133</v>
-      </c>
-      <c r="H178" s="17"/>
-      <c r="I178" s="17"/>
-      <c r="J178" s="17"/>
+      <c r="G178" s="30" t="s">
+        <v>155</v>
+      </c>
+      <c r="H178" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="I178" s="17">
+        <v>2</v>
+      </c>
+      <c r="J178" s="30">
+        <v>55080</v>
+      </c>
       <c r="K178" s="17"/>
       <c r="L178" s="17"/>
       <c r="M178" s="17"/>
@@ -50821,57 +50819,61 @@
       <c r="C179"/>
       <c r="D179"/>
       <c r="G179"/>
+      <c r="H179"/>
     </row>
     <row r="180" spans="1:1025">
       <c r="A180" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B180" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C180" s="14">
         <v>2</v>
       </c>
       <c r="D180" s="18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G180" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="H180"/>
     </row>
     <row r="181" spans="1:1025">
       <c r="A181" s="14" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B181" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C181" s="14">
         <v>2</v>
       </c>
       <c r="D181" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G181" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="H181"/>
     </row>
     <row r="182" spans="1:1025">
       <c r="A182" s="14" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B182" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C182" s="14">
         <v>2</v>
       </c>
       <c r="D182" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="G182" s="30" t="s">
-        <v>136</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="H182"/>
     </row>
     <row r="183" spans="1:1025">
       <c r="A183"/>
@@ -50879,108 +50881,130 @@
       <c r="C183"/>
       <c r="D183" s="18"/>
       <c r="G183" s="30"/>
+      <c r="H183"/>
     </row>
     <row r="184" spans="1:1025">
       <c r="A184" s="14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B184" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C184" s="14">
         <v>2</v>
       </c>
       <c r="D184" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="G184" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H184"/>
     </row>
     <row r="185" spans="1:1025">
       <c r="A185" s="14" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B185" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C185" s="14">
         <v>2</v>
       </c>
       <c r="D185" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G185" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H185"/>
     </row>
     <row r="186" spans="1:1025">
       <c r="A186" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C186" s="14">
         <v>2</v>
       </c>
       <c r="D186" s="18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="G186" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H186"/>
     </row>
     <row r="187" spans="1:1025">
       <c r="A187" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B187" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C187" s="14">
         <v>2</v>
       </c>
       <c r="D187" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G187" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H187"/>
     </row>
     <row r="188" spans="1:1025">
       <c r="A188" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B188" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C188" s="14">
         <v>2</v>
       </c>
       <c r="D188" s="18" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G188" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H188"/>
     </row>
     <row r="189" spans="1:1025">
       <c r="A189" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B189" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C189" s="14">
         <v>2</v>
       </c>
       <c r="D189" s="18" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G189" s="30" t="s">
-        <v>143</v>
-      </c>
+        <v>141</v>
+      </c>
+      <c r="H189"/>
+    </row>
+    <row r="190" spans="1:1025">
+      <c r="H190"/>
+    </row>
+    <row r="191" spans="1:1025">
+      <c r="H191"/>
+    </row>
+    <row r="192" spans="1:1025">
+      <c r="H192"/>
+    </row>
+    <row r="193" spans="8:8">
+      <c r="H193"/>
+    </row>
+    <row r="194" spans="8:8">
+      <c r="H194"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -51001,7 +51025,7 @@
       <selection sqref="A1:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -60175,7 +60199,7 @@
       <selection sqref="A1:XFD81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -69349,7 +69373,7 @@
       <selection sqref="A1:XFD83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">
@@ -78746,10 +78770,10 @@
   <dimension ref="A1:AK83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD83"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:37">
       <c r="A1">

</xml_diff>